<commit_message>
Fixing errors found as boxplot outliers
</commit_message>
<xml_diff>
--- a/Data/phenotypic data/RawData/2012 Data/BogUpper5-R9.xlsx
+++ b/Data/phenotypic data/RawData/2012 Data/BogUpper5-R9.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="240" windowWidth="25440" windowHeight="18020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1475,8 +1475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:W784"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A740" workbookViewId="0">
-      <selection activeCell="V775" sqref="V775"/>
+    <sheetView tabSelected="1" topLeftCell="A319" workbookViewId="0">
+      <selection activeCell="L348" sqref="L348"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -22037,7 +22037,7 @@
         <v>25.9</v>
       </c>
       <c r="L348" s="35">
-        <v>1739</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="M348" s="35">
         <v>3.1360000000000001</v>
@@ -47696,6 +47696,78 @@
     </row>
   </sheetData>
   <mergeCells count="81">
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="K34:M34"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="O62:P62"/>
+    <mergeCell ref="K63:M63"/>
+    <mergeCell ref="Q63:R63"/>
+    <mergeCell ref="O91:P91"/>
+    <mergeCell ref="K92:M92"/>
+    <mergeCell ref="Q92:R92"/>
+    <mergeCell ref="O120:P120"/>
+    <mergeCell ref="K121:M121"/>
+    <mergeCell ref="Q121:R121"/>
+    <mergeCell ref="O149:P149"/>
+    <mergeCell ref="K150:M150"/>
+    <mergeCell ref="Q150:R150"/>
+    <mergeCell ref="O178:P178"/>
+    <mergeCell ref="K179:M179"/>
+    <mergeCell ref="Q179:R179"/>
+    <mergeCell ref="O207:P207"/>
+    <mergeCell ref="K208:M208"/>
+    <mergeCell ref="Q208:R208"/>
+    <mergeCell ref="O236:P236"/>
+    <mergeCell ref="K237:M237"/>
+    <mergeCell ref="Q237:R237"/>
+    <mergeCell ref="O265:P265"/>
+    <mergeCell ref="K266:M266"/>
+    <mergeCell ref="Q266:R266"/>
+    <mergeCell ref="O294:P294"/>
+    <mergeCell ref="K295:M295"/>
+    <mergeCell ref="Q295:R295"/>
+    <mergeCell ref="O323:P323"/>
+    <mergeCell ref="K324:M324"/>
+    <mergeCell ref="Q324:R324"/>
+    <mergeCell ref="O352:P352"/>
+    <mergeCell ref="K353:M353"/>
+    <mergeCell ref="Q353:R353"/>
+    <mergeCell ref="O381:P381"/>
+    <mergeCell ref="K382:M382"/>
+    <mergeCell ref="Q382:R382"/>
+    <mergeCell ref="O410:P410"/>
+    <mergeCell ref="K411:M411"/>
+    <mergeCell ref="Q411:R411"/>
+    <mergeCell ref="O439:P439"/>
+    <mergeCell ref="K440:M440"/>
+    <mergeCell ref="Q440:R440"/>
+    <mergeCell ref="O468:P468"/>
+    <mergeCell ref="K469:M469"/>
+    <mergeCell ref="Q469:R469"/>
+    <mergeCell ref="O497:P497"/>
+    <mergeCell ref="K498:M498"/>
+    <mergeCell ref="Q498:R498"/>
+    <mergeCell ref="O526:P526"/>
+    <mergeCell ref="K527:M527"/>
+    <mergeCell ref="Q527:R527"/>
+    <mergeCell ref="O555:P555"/>
+    <mergeCell ref="K556:M556"/>
+    <mergeCell ref="Q556:R556"/>
+    <mergeCell ref="O584:P584"/>
+    <mergeCell ref="K585:M585"/>
+    <mergeCell ref="Q585:R585"/>
+    <mergeCell ref="O613:P613"/>
+    <mergeCell ref="K614:M614"/>
+    <mergeCell ref="Q614:R614"/>
+    <mergeCell ref="O642:P642"/>
+    <mergeCell ref="K643:M643"/>
+    <mergeCell ref="Q643:R643"/>
+    <mergeCell ref="O671:P671"/>
+    <mergeCell ref="K672:M672"/>
+    <mergeCell ref="Q672:R672"/>
     <mergeCell ref="O758:P758"/>
     <mergeCell ref="K759:M759"/>
     <mergeCell ref="Q759:R759"/>
@@ -47705,78 +47777,6 @@
     <mergeCell ref="O729:P729"/>
     <mergeCell ref="K730:M730"/>
     <mergeCell ref="Q730:R730"/>
-    <mergeCell ref="O642:P642"/>
-    <mergeCell ref="K643:M643"/>
-    <mergeCell ref="Q643:R643"/>
-    <mergeCell ref="O671:P671"/>
-    <mergeCell ref="K672:M672"/>
-    <mergeCell ref="Q672:R672"/>
-    <mergeCell ref="O584:P584"/>
-    <mergeCell ref="K585:M585"/>
-    <mergeCell ref="Q585:R585"/>
-    <mergeCell ref="O613:P613"/>
-    <mergeCell ref="K614:M614"/>
-    <mergeCell ref="Q614:R614"/>
-    <mergeCell ref="O526:P526"/>
-    <mergeCell ref="K527:M527"/>
-    <mergeCell ref="Q527:R527"/>
-    <mergeCell ref="O555:P555"/>
-    <mergeCell ref="K556:M556"/>
-    <mergeCell ref="Q556:R556"/>
-    <mergeCell ref="O468:P468"/>
-    <mergeCell ref="K469:M469"/>
-    <mergeCell ref="Q469:R469"/>
-    <mergeCell ref="O497:P497"/>
-    <mergeCell ref="K498:M498"/>
-    <mergeCell ref="Q498:R498"/>
-    <mergeCell ref="O410:P410"/>
-    <mergeCell ref="K411:M411"/>
-    <mergeCell ref="Q411:R411"/>
-    <mergeCell ref="O439:P439"/>
-    <mergeCell ref="K440:M440"/>
-    <mergeCell ref="Q440:R440"/>
-    <mergeCell ref="O352:P352"/>
-    <mergeCell ref="K353:M353"/>
-    <mergeCell ref="Q353:R353"/>
-    <mergeCell ref="O381:P381"/>
-    <mergeCell ref="K382:M382"/>
-    <mergeCell ref="Q382:R382"/>
-    <mergeCell ref="O294:P294"/>
-    <mergeCell ref="K295:M295"/>
-    <mergeCell ref="Q295:R295"/>
-    <mergeCell ref="O323:P323"/>
-    <mergeCell ref="K324:M324"/>
-    <mergeCell ref="Q324:R324"/>
-    <mergeCell ref="O236:P236"/>
-    <mergeCell ref="K237:M237"/>
-    <mergeCell ref="Q237:R237"/>
-    <mergeCell ref="O265:P265"/>
-    <mergeCell ref="K266:M266"/>
-    <mergeCell ref="Q266:R266"/>
-    <mergeCell ref="O178:P178"/>
-    <mergeCell ref="K179:M179"/>
-    <mergeCell ref="Q179:R179"/>
-    <mergeCell ref="O207:P207"/>
-    <mergeCell ref="K208:M208"/>
-    <mergeCell ref="Q208:R208"/>
-    <mergeCell ref="O120:P120"/>
-    <mergeCell ref="K121:M121"/>
-    <mergeCell ref="Q121:R121"/>
-    <mergeCell ref="O149:P149"/>
-    <mergeCell ref="K150:M150"/>
-    <mergeCell ref="Q150:R150"/>
-    <mergeCell ref="O62:P62"/>
-    <mergeCell ref="K63:M63"/>
-    <mergeCell ref="Q63:R63"/>
-    <mergeCell ref="O91:P91"/>
-    <mergeCell ref="K92:M92"/>
-    <mergeCell ref="Q92:R92"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="K34:M34"/>
-    <mergeCell ref="Q34:R34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>